<commit_message>
[DESC]: Add batter charger to inverntory
</commit_message>
<xml_diff>
--- a/r1_test_command_list_tag1.2.xlsx
+++ b/r1_test_command_list_tag1.2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="216">
   <si>
     <t>./inventory.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Device shutdown</t>
-  </si>
-  <si>
-    <t>Check I2C bus chip state, chips list defined at i2c.conf</t>
   </si>
   <si>
     <t>Get bluetooth MAC address</t>
@@ -382,10 +379,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>get_temperature.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>set_battery_poweron.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -446,9 +439,6 @@
   </si>
   <si>
     <t>FeedBack from RD</t>
-  </si>
-  <si>
-    <t>Added</t>
   </si>
   <si>
     <t>"OK" in the end of the log is a sign of successful BT set operation.</t>
@@ -728,12 +718,6 @@
     <t>get_bat_sw_ver.sh</t>
   </si>
   <si>
-    <t>Added in 1.1.6. A requirement for a battery o shutdown after a command is "no power supplied oto the battery". If usb cable is connected it is not supposed to go to shutdown mode. But on our side it goes even with usb cable attached, we are not yet sure why this happens. A proper method to shutdown a battery is still under nvestigation. Maybe we will use this added script or swithc to some button long press.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">git </t>
-  </si>
-  <si>
     <t>get_bat_temp.sh</t>
   </si>
   <si>
@@ -774,6 +758,30 @@
   </si>
   <si>
     <t>adb shell /etc/factory-test/r1/get_bat_temp.sh</t>
+  </si>
+  <si>
+    <t>Added shared with email</t>
+  </si>
+  <si>
+    <t>Check I2C bus ICs state</t>
+  </si>
+  <si>
+    <t>get_amp1_temp.sh</t>
+  </si>
+  <si>
+    <t>get_amp2_temp.sh</t>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/get_amp1_temp.sh</t>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/get_amp2_temp.sh</t>
+  </si>
+  <si>
+    <t>Added in 1.1.6. Amplifier 1 temperature</t>
+  </si>
+  <si>
+    <t>Added in 1.1.6. Amplifier 2 temperature</t>
   </si>
 </sst>
 </file>
@@ -974,7 +982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1036,7 +1044,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1056,9 +1064,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1364,7 +1369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -1375,8 +1380,8 @@
     <col min="1" max="1" width="6.85546875" style="14" customWidth="1"/>
     <col min="2" max="2" width="6" style="22" customWidth="1"/>
     <col min="3" max="3" width="37" style="14" customWidth="1"/>
-    <col min="4" max="4" width="46.5703125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="46.7109375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="14" customWidth="1"/>
     <col min="6" max="7" width="5.85546875" style="14" customWidth="1"/>
     <col min="8" max="8" width="79.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="14"/>
@@ -1384,113 +1389,113 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A1" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>131</v>
-      </c>
       <c r="G1" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="32">
+        <v>122</v>
+      </c>
+      <c r="B2" s="25">
         <v>1</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>12</v>
+        <v>87</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" customHeight="1">
       <c r="A3" s="26"/>
-      <c r="B3" s="32">
+      <c r="B3" s="25">
         <v>2</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>15</v>
+        <v>127</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="26"/>
-      <c r="B4" s="32">
+      <c r="B4" s="25">
         <v>3</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>115</v>
+        <v>85</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>113</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="26"/>
-      <c r="B5" s="32">
+      <c r="B5" s="25">
         <v>4</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>116</v>
+        <v>86</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
@@ -1498,17 +1503,17 @@
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="26"/>
-      <c r="B6" s="32">
+      <c r="B6" s="25">
         <v>5</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>9</v>
+        <v>139</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>8</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -1516,17 +1521,17 @@
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="26"/>
-      <c r="B7" s="32">
+      <c r="B7" s="25">
         <v>6</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>14</v>
+        <v>84</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>13</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -1534,17 +1539,17 @@
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="26"/>
-      <c r="B8" s="32">
+      <c r="B8" s="25">
         <v>7</v>
       </c>
       <c r="C8" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>156</v>
+      <c r="E8" s="24" t="s">
+        <v>153</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -1552,125 +1557,125 @@
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="26"/>
-      <c r="B9" s="32">
+      <c r="B9" s="25">
         <v>8</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>8</v>
+        <v>89</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>209</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" ht="56.25" customHeight="1">
+    <row r="10" spans="1:8" ht="50.25" customHeight="1">
       <c r="A10" s="26"/>
-      <c r="B10" s="32">
+      <c r="B10" s="25">
         <v>9</v>
       </c>
       <c r="C10" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>13</v>
+      <c r="E10" s="23" t="s">
+        <v>12</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G10" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="22.5" customHeight="1">
+      <c r="A11" s="26"/>
+      <c r="B11" s="25">
+        <v>10</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="H10" s="10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
-      <c r="A11" s="26"/>
-      <c r="B11" s="32">
-        <v>10</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>96</v>
-      </c>
       <c r="H11" s="10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="26"/>
-      <c r="B12" s="32">
+      <c r="B12" s="25">
         <v>11</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>11</v>
+        <v>83</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>10</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G12" s="18"/>
       <c r="H12" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="26"/>
-      <c r="B13" s="32">
+      <c r="B13" s="25">
         <v>12</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>93</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>94</v>
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
+    <row r="14" spans="1:8" ht="22.5" customHeight="1">
       <c r="A14" s="26"/>
-      <c r="B14" s="32">
+      <c r="B14" s="25">
         <v>13</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>10</v>
+        <v>136</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>9</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
@@ -1678,22 +1683,22 @@
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" s="26"/>
-      <c r="B15" s="32">
+      <c r="B15" s="25">
         <v>14</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>169</v>
+        <v>146</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>166</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
       <c r="H15" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1">
@@ -1702,11 +1707,11 @@
         <v>15</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" s="23"/>
-      <c r="E16" s="17" t="s">
-        <v>157</v>
+      <c r="E16" s="23" t="s">
+        <v>154</v>
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
@@ -1718,15 +1723,19 @@
         <v>16</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="17" t="s">
-        <v>158</v>
+        <v>210</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>155</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
-      <c r="H17" s="12"/>
+      <c r="H17" s="10" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
       <c r="A18" s="26"/>
@@ -1734,15 +1743,19 @@
         <v>17</v>
       </c>
       <c r="C18" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="E18" s="23" t="s">
         <v>155</v>
-      </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="17" t="s">
-        <v>170</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
-      <c r="H18" s="12"/>
+      <c r="H18" s="10" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="25.5" customHeight="1">
       <c r="A19" s="26"/>
@@ -1750,234 +1763,230 @@
         <v>18</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>208</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>171</v>
+        <v>152</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23" t="s">
+        <v>167</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
-      <c r="H19" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1">
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20" spans="1:8" ht="25.5" customHeight="1">
       <c r="A20" s="26"/>
       <c r="B20" s="25">
         <v>19</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>159</v>
+        <v>203</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>168</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
       <c r="H20" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1">
       <c r="A21" s="26"/>
-      <c r="B21" s="32">
+      <c r="B21" s="25">
         <v>20</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>160</v>
+        <v>204</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>156</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
       <c r="H21" s="10" t="s">
-        <v>189</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1">
       <c r="A22" s="26"/>
-      <c r="B22" s="32">
+      <c r="B22" s="25">
         <v>21</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="E22" s="17" t="s">
-        <v>161</v>
+      <c r="E22" s="23" t="s">
+        <v>157</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
       <c r="H22" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1">
       <c r="A23" s="26"/>
-      <c r="B23" s="32">
+      <c r="B23" s="25">
         <v>22</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>162</v>
+        <v>200</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>158</v>
       </c>
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
       <c r="H23" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
       <c r="A24" s="26"/>
-      <c r="B24" s="32">
+      <c r="B24" s="25">
         <v>23</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>163</v>
+        <v>199</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
       <c r="H24" s="10" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="81" customHeight="1">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" customHeight="1">
       <c r="A25" s="26"/>
-      <c r="B25" s="32">
+      <c r="B25" s="25">
         <v>24</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>172</v>
+        <v>198</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>160</v>
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="26"/>
+      <c r="B26" s="25">
+        <v>25</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="D26" s="23" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="32">
-        <v>25</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="17" t="s">
-        <v>173</v>
+      <c r="E26" s="23" t="s">
+        <v>169</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
-      <c r="H26" s="11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="30">
+      <c r="H26" s="10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="31.5" customHeight="1">
       <c r="A27" s="26"/>
-      <c r="B27" s="32">
+      <c r="B27" s="25">
         <v>26</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>164</v>
+        <v>99</v>
+      </c>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23" t="s">
+        <v>170</v>
       </c>
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
-      <c r="H27" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1">
+      <c r="H27" s="11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30">
       <c r="A28" s="26"/>
-      <c r="B28" s="32">
+      <c r="B28" s="25">
         <v>27</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="17" t="s">
-        <v>165</v>
+        <v>195</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>161</v>
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
-      <c r="H28" s="11" t="s">
-        <v>191</v>
+      <c r="H28" s="10" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1">
       <c r="A29" s="26"/>
-      <c r="B29" s="32">
+      <c r="B29" s="25">
         <v>28</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="D29" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>166</v>
+        <v>185</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23" t="s">
+        <v>162</v>
       </c>
       <c r="F29" s="18"/>
       <c r="G29" s="18"/>
-      <c r="H29" s="10" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1">
+      <c r="H29" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="26.25" customHeight="1">
       <c r="A30" s="26"/>
       <c r="B30" s="25">
         <v>29</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>153</v>
+        <v>194</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>102</v>
+        <v>207</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>163</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
       <c r="H30" s="10" t="s">
-        <v>135</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1">
@@ -1986,16 +1995,18 @@
         <v>30</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="17" t="s">
-        <v>183</v>
+        <v>150</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
-      <c r="H31" s="11" t="s">
-        <v>127</v>
+      <c r="H31" s="10" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1">
@@ -2004,35 +2015,33 @@
         <v>31</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="D32" s="23"/>
-      <c r="E32" s="17" t="s">
-        <v>174</v>
+      <c r="E32" s="23" t="s">
+        <v>180</v>
       </c>
       <c r="F32" s="18"/>
       <c r="G32" s="18"/>
-      <c r="H32" s="12"/>
-    </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1">
+      <c r="H32" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="25.5" customHeight="1">
       <c r="A33" s="26"/>
       <c r="B33" s="25">
         <v>32</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>175</v>
+        <v>101</v>
+      </c>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23" t="s">
+        <v>171</v>
       </c>
       <c r="F33" s="18"/>
       <c r="G33" s="18"/>
-      <c r="H33" s="10" t="s">
-        <v>135</v>
-      </c>
+      <c r="H33" s="12"/>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1">
       <c r="A34" s="26"/>
@@ -2040,18 +2049,18 @@
         <v>33</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>167</v>
+        <v>147</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>172</v>
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="18"/>
       <c r="H34" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1">
@@ -2060,15 +2069,19 @@
         <v>34</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="17" t="s">
-        <v>176</v>
+        <v>134</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>164</v>
       </c>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
-      <c r="H35" s="12"/>
+      <c r="H35" s="10" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1">
       <c r="A36" s="26"/>
@@ -2076,43 +2089,43 @@
         <v>35</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D36" s="23"/>
-      <c r="E36" s="17" t="s">
-        <v>177</v>
+      <c r="E36" s="23" t="s">
+        <v>173</v>
       </c>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
       <c r="H36" s="12"/>
     </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1">
+    <row r="37" spans="1:8" ht="27" customHeight="1">
       <c r="A37" s="26"/>
       <c r="B37" s="25">
         <v>36</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D37" s="23"/>
-      <c r="E37" s="17" t="s">
-        <v>178</v>
+      <c r="E37" s="23" t="s">
+        <v>174</v>
       </c>
       <c r="F37" s="18"/>
       <c r="G37" s="18"/>
       <c r="H37" s="12"/>
     </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1">
+    <row r="38" spans="1:8" ht="39" customHeight="1">
       <c r="A38" s="26"/>
       <c r="B38" s="25">
         <v>37</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D38" s="23"/>
-      <c r="E38" s="17" t="s">
-        <v>179</v>
+      <c r="E38" s="23" t="s">
+        <v>175</v>
       </c>
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
@@ -2124,11 +2137,11 @@
         <v>38</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D39" s="23"/>
-      <c r="E39" s="17" t="s">
-        <v>168</v>
+      <c r="E39" s="23" t="s">
+        <v>176</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="18"/>
@@ -2140,11 +2153,11 @@
         <v>39</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="D40" s="24"/>
-      <c r="E40" s="17" t="s">
-        <v>180</v>
+        <v>106</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23" t="s">
+        <v>165</v>
       </c>
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
@@ -2156,11 +2169,11 @@
         <v>40</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D41" s="24"/>
-      <c r="E41" s="17" t="s">
-        <v>181</v>
+      <c r="E41" s="23" t="s">
+        <v>177</v>
       </c>
       <c r="F41" s="18"/>
       <c r="G41" s="18"/>
@@ -2172,65 +2185,81 @@
         <v>41</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D42" s="24"/>
-      <c r="E42" s="17" t="s">
-        <v>182</v>
+      <c r="E42" s="23" t="s">
+        <v>178</v>
       </c>
       <c r="F42" s="18"/>
       <c r="G42" s="18"/>
       <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1">
-      <c r="A43" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="B43" s="32">
-        <v>1</v>
+      <c r="A43" s="26"/>
+      <c r="B43" s="25">
+        <v>42</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="D43" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="E43" s="18" t="s">
-        <v>184</v>
+        <v>109</v>
+      </c>
+      <c r="D43" s="24"/>
+      <c r="E43" s="23" t="s">
+        <v>179</v>
       </c>
       <c r="F43" s="18"/>
       <c r="G43" s="18"/>
-      <c r="H43" s="10" t="s">
+      <c r="H43" s="12"/>
+    </row>
+    <row r="44" spans="1:8" ht="15" customHeight="1">
+      <c r="A44" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="25">
+        <v>1</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D44" s="24" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="15" customHeight="1">
-      <c r="A44" s="26"/>
-      <c r="B44" s="32">
-        <v>2</v>
-      </c>
-      <c r="C44" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="D44" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>186</v>
+      <c r="E44" s="24" t="s">
+        <v>181</v>
       </c>
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
       <c r="H44" s="10" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4">
-      <c r="D49"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15" customHeight="1">
+      <c r="A45" s="26"/>
+      <c r="B45" s="25">
+        <v>2</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4">
+      <c r="D50"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A42"/>
-    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A2:A43"/>
+    <mergeCell ref="A44:A45"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2259,375 +2288,375 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="31"/>
       <c r="B2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="31"/>
       <c r="B3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="31"/>
       <c r="B5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="31"/>
       <c r="B6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="31"/>
       <c r="B8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="31"/>
       <c r="B9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="31"/>
       <c r="B11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="31"/>
       <c r="B12" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="31"/>
       <c r="B14" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="31"/>
       <c r="B15" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="30"/>
       <c r="B17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="30"/>
       <c r="B18" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="30"/>
       <c r="B20" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="30"/>
       <c r="B21" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="30"/>
       <c r="B23" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="28"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="30"/>
       <c r="B24" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="28"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="30"/>
       <c r="B25" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="28"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="30"/>
       <c r="B26" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="28"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="30"/>
       <c r="B27" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" s="28"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="30"/>
       <c r="B28" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="28"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="30"/>
       <c r="B29" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="28"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="28"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="30"/>
       <c r="B31" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" s="28"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="30"/>
       <c r="B32" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" s="28"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="30"/>
       <c r="B33" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" s="28"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="30"/>
       <c r="B34" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" s="28"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="30"/>
       <c r="B35" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C35" s="28"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="30"/>
       <c r="B36" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36" s="28"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="30"/>
       <c r="B37" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C37" s="28"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" s="28"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="30"/>
       <c r="B39" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C39" s="28"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="30"/>
       <c r="B40" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="28"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="30"/>
       <c r="B41" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C41" s="28"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="30"/>
       <c r="B42" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="28"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="30"/>
       <c r="B43" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C43" s="28"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="30"/>
       <c r="B44" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C44" s="28"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="30"/>
       <c r="B45" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="28"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C46" s="28"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="30"/>
       <c r="B47" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C47" s="28"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="30"/>
       <c r="B48" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C48" s="28"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="30"/>
       <c r="B49" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C49" s="28"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="30"/>
       <c r="B50" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C50" s="28"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="30"/>
       <c r="B51" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C51" s="28"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="30"/>
       <c r="B52" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C52" s="28"/>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="30"/>
       <c r="B53" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C53" s="29"/>
     </row>

</xml_diff>